<commit_message>
new analysis without residuals (lm, censored, survival, cox and repeatability) + starting permanova behaviour by time
</commit_message>
<xml_diff>
--- a/Snake_captures.xlsx
+++ b/Snake_captures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc9\Desktop\Marc\CREAF\Snake tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207741BA-E1A0-4F0F-B2F5-8F7A30D735E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3102D8A-2542-492B-9F40-6FE8A4510623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01147B77-2702-4854-93BF-07D9F62605BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{01147B77-2702-4854-93BF-07D9F62605BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Snakes" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Snakes!$A$1:$AX$131</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1999" uniqueCount="196">
   <si>
     <t>Snake_ID</t>
   </si>
@@ -626,6 +627,9 @@
   <si>
     <t>It went and refuged between wall and refuge. Sexing with clip probably was wrong though perforation</t>
   </si>
+  <si>
+    <t xml:space="preserve"> the tag is separated, and as the sanke didn't get out of the refuge, we can't determine its visual phenotype in the video. I think this snake is SN_1, as it is the only snake without tag in the behaviour bag, but I cannot confirm.</t>
+  </si>
 </sst>
 </file>
 
@@ -1107,10 +1111,10 @@
   <dimension ref="A1:AZ131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN40" sqref="AN40"/>
+      <selection pane="bottomRight" activeCell="AO5" sqref="AO5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5026,7 +5030,7 @@
         <v>102.39</v>
       </c>
       <c r="AM32">
-        <f t="shared" ref="AM32:AM33" si="43">AL32-AR32</f>
+        <f t="shared" ref="AM32:AM36" si="43">AL32-AR32</f>
         <v>101.39</v>
       </c>
       <c r="AN32" s="50">
@@ -5146,7 +5150,7 @@
         <v>110.6</v>
       </c>
       <c r="AJ33">
-        <f t="shared" ref="AJ33" si="44">AI33-AK33</f>
+        <f t="shared" ref="AJ33:AJ36" si="44">AI33-AK33</f>
         <v>24.699999999999989</v>
       </c>
       <c r="AK33">
@@ -5160,7 +5164,7 @@
         <v>122.5</v>
       </c>
       <c r="AN33" s="50">
-        <f t="shared" ref="AN33" si="45">LOG(AM33)/LOG(AK33)</f>
+        <f t="shared" ref="AN33:AN36" si="45">LOG(AM33)/LOG(AK33)</f>
         <v>1.0797018974792816</v>
       </c>
       <c r="AO33">
@@ -5272,21 +5276,54 @@
       <c r="AF34" s="1"/>
       <c r="AG34" s="1"/>
       <c r="AH34" s="1"/>
-      <c r="AI34" s="1"/>
-      <c r="AJ34" s="1"/>
-      <c r="AK34" s="1"/>
-      <c r="AL34" s="1"/>
-      <c r="AM34" s="1"/>
-      <c r="AN34" s="1"/>
-      <c r="AO34" s="1"/>
-      <c r="AP34" s="1"/>
-      <c r="AQ34" s="1"/>
-      <c r="AR34" s="1"/>
-      <c r="AS34" s="1"/>
-      <c r="AT34" s="1"/>
-      <c r="AU34" s="1"/>
-      <c r="AV34" s="1"/>
-      <c r="AW34" s="1"/>
+      <c r="AI34">
+        <v>68</v>
+      </c>
+      <c r="AJ34">
+        <f t="shared" si="44"/>
+        <v>14.600000000000001</v>
+      </c>
+      <c r="AK34">
+        <v>53.4</v>
+      </c>
+      <c r="AL34">
+        <v>32.549999999999997</v>
+      </c>
+      <c r="AM34">
+        <f t="shared" si="43"/>
+        <v>31.549999999999997</v>
+      </c>
+      <c r="AN34" s="50">
+        <f t="shared" si="45"/>
+        <v>0.86770683911682378</v>
+      </c>
+      <c r="AO34">
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <v>13</v>
+      </c>
+      <c r="AQ34" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR34">
+        <v>1</v>
+      </c>
+      <c r="AS34" t="s">
+        <v>180</v>
+      </c>
+      <c r="AT34">
+        <v>0</v>
+      </c>
+      <c r="AU34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV34" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW34" t="s">
+        <v>33</v>
+      </c>
       <c r="AX34" s="1"/>
       <c r="AY34" s="1">
         <v>1</v>
@@ -5367,21 +5404,54 @@
       <c r="AF35" s="14"/>
       <c r="AG35" s="14"/>
       <c r="AH35" s="14"/>
-      <c r="AI35" s="14"/>
-      <c r="AJ35" s="14"/>
-      <c r="AK35" s="14"/>
-      <c r="AL35" s="14"/>
-      <c r="AM35" s="14"/>
-      <c r="AN35" s="14"/>
-      <c r="AO35" s="14"/>
-      <c r="AP35" s="14"/>
-      <c r="AQ35" s="14"/>
-      <c r="AR35" s="14"/>
-      <c r="AS35" s="14"/>
-      <c r="AT35" s="14"/>
-      <c r="AU35" s="14"/>
-      <c r="AV35" s="14"/>
-      <c r="AW35" s="14"/>
+      <c r="AI35">
+        <v>96.1</v>
+      </c>
+      <c r="AJ35">
+        <f t="shared" si="44"/>
+        <v>21.899999999999991</v>
+      </c>
+      <c r="AK35">
+        <v>74.2</v>
+      </c>
+      <c r="AL35">
+        <v>75.760000000000005</v>
+      </c>
+      <c r="AM35">
+        <f t="shared" si="43"/>
+        <v>74.760000000000005</v>
+      </c>
+      <c r="AN35" s="50">
+        <f t="shared" si="45"/>
+        <v>1.0017458194021895</v>
+      </c>
+      <c r="AO35">
+        <v>0</v>
+      </c>
+      <c r="AP35">
+        <v>8</v>
+      </c>
+      <c r="AQ35" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR35">
+        <v>1</v>
+      </c>
+      <c r="AS35" t="s">
+        <v>180</v>
+      </c>
+      <c r="AT35">
+        <v>0</v>
+      </c>
+      <c r="AU35" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV35" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW35" t="s">
+        <v>33</v>
+      </c>
       <c r="AX35" s="14"/>
       <c r="AY35" s="14">
         <v>1</v>
@@ -5464,21 +5534,54 @@
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
       <c r="AH36" s="1"/>
-      <c r="AI36" s="1"/>
-      <c r="AJ36" s="1"/>
-      <c r="AK36" s="1"/>
-      <c r="AL36" s="1"/>
-      <c r="AM36" s="1"/>
-      <c r="AN36" s="1"/>
-      <c r="AO36" s="1"/>
-      <c r="AP36" s="1"/>
-      <c r="AQ36" s="1"/>
-      <c r="AR36" s="1"/>
-      <c r="AS36" s="1"/>
-      <c r="AT36" s="1"/>
-      <c r="AU36" s="1"/>
-      <c r="AV36" s="1"/>
-      <c r="AW36" s="1"/>
+      <c r="AI36">
+        <v>77.2</v>
+      </c>
+      <c r="AJ36">
+        <f t="shared" si="44"/>
+        <v>5.9000000000000057</v>
+      </c>
+      <c r="AK36">
+        <v>71.3</v>
+      </c>
+      <c r="AL36">
+        <v>59.72</v>
+      </c>
+      <c r="AM36">
+        <f t="shared" si="43"/>
+        <v>58.72</v>
+      </c>
+      <c r="AN36" s="50">
+        <f t="shared" si="45"/>
+        <v>0.95450652459809082</v>
+      </c>
+      <c r="AO36">
+        <v>1</v>
+      </c>
+      <c r="AP36">
+        <v>1</v>
+      </c>
+      <c r="AQ36" t="s">
+        <v>185</v>
+      </c>
+      <c r="AR36">
+        <v>1</v>
+      </c>
+      <c r="AS36" t="s">
+        <v>179</v>
+      </c>
+      <c r="AT36">
+        <v>0</v>
+      </c>
+      <c r="AU36" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV36" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW36" t="s">
+        <v>33</v>
+      </c>
       <c r="AX36" s="1"/>
       <c r="AY36" s="1">
         <v>1</v>
@@ -6421,7 +6524,7 @@
         <v>53.7</v>
       </c>
       <c r="AJ43" s="11">
-        <f t="shared" ref="AJ43:AJ45" si="65">AI43-AK43</f>
+        <f t="shared" ref="AJ43:AJ46" si="65">AI43-AK43</f>
         <v>10.700000000000003</v>
       </c>
       <c r="AK43" s="11">
@@ -6431,7 +6534,7 @@
         <v>14.5</v>
       </c>
       <c r="AM43" s="11">
-        <f t="shared" ref="AM43:AM45" si="66">AL43-AR43</f>
+        <f t="shared" ref="AM43:AM46" si="66">AL43-AR43</f>
         <v>13.5</v>
       </c>
       <c r="AN43" s="11">
@@ -6600,7 +6703,7 @@
         <v>55.5</v>
       </c>
       <c r="AN44" s="50">
-        <f t="shared" ref="AN44:AN45" si="68">LOG(AM44)/LOG(AK44)</f>
+        <f t="shared" ref="AN44:AN46" si="68">LOG(AM44)/LOG(AK44)</f>
         <v>0.94036375945673856</v>
       </c>
       <c r="AO44">
@@ -6906,11 +7009,54 @@
       <c r="AH46">
         <v>10782.722811338501</v>
       </c>
-      <c r="AI46"/>
-      <c r="AJ46"/>
-      <c r="AO46"/>
-      <c r="AP46"/>
-      <c r="AQ46"/>
+      <c r="AI46">
+        <v>93.2</v>
+      </c>
+      <c r="AJ46">
+        <f t="shared" si="65"/>
+        <v>20.900000000000006</v>
+      </c>
+      <c r="AK46">
+        <v>72.3</v>
+      </c>
+      <c r="AL46">
+        <v>76.02</v>
+      </c>
+      <c r="AM46">
+        <f t="shared" si="66"/>
+        <v>75.02</v>
+      </c>
+      <c r="AN46" s="50">
+        <f t="shared" si="68"/>
+        <v>1.0086269873217679</v>
+      </c>
+      <c r="AO46">
+        <v>0</v>
+      </c>
+      <c r="AP46">
+        <v>2</v>
+      </c>
+      <c r="AQ46" t="s">
+        <v>185</v>
+      </c>
+      <c r="AR46">
+        <v>1</v>
+      </c>
+      <c r="AS46" t="s">
+        <v>179</v>
+      </c>
+      <c r="AT46">
+        <v>0</v>
+      </c>
+      <c r="AU46" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV46" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW46" t="s">
+        <v>33</v>
+      </c>
       <c r="AY46">
         <v>2</v>
       </c>
@@ -9649,7 +9795,9 @@
       <c r="AP63">
         <v>10</v>
       </c>
-      <c r="AQ63"/>
+      <c r="AQ63" t="s">
+        <v>184</v>
+      </c>
       <c r="AR63">
         <v>1</v>
       </c>
@@ -10730,13 +10878,13 @@
       </c>
       <c r="AT70"/>
       <c r="AU70" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AV70" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AW70" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AY70" s="35">
         <v>2</v>
@@ -10854,7 +11002,7 @@
         <v>84</v>
       </c>
       <c r="AJ71">
-        <f t="shared" ref="AJ71" si="113">AI71-AK71</f>
+        <f t="shared" ref="AJ71:AJ72" si="113">AI71-AK71</f>
         <v>18.799999999999997</v>
       </c>
       <c r="AK71">
@@ -10864,11 +11012,11 @@
         <v>80.400000000000006</v>
       </c>
       <c r="AM71">
-        <f t="shared" ref="AM71" si="114">AL71-AR71</f>
+        <f t="shared" ref="AM71:AM72" si="114">AL71-AR71</f>
         <v>77.650000000000006</v>
       </c>
       <c r="AN71" s="50">
-        <f t="shared" ref="AN71" si="115">LOG(AM71)/LOG(AK71)</f>
+        <f t="shared" ref="AN71:AN72" si="115">LOG(AM71)/LOG(AK71)</f>
         <v>1.0418321427081949</v>
       </c>
       <c r="AO71">
@@ -11010,13 +11158,59 @@
       <c r="AH72">
         <v>10010.747589042699</v>
       </c>
-      <c r="AI72"/>
-      <c r="AJ72"/>
-      <c r="AO72"/>
-      <c r="AP72"/>
-      <c r="AQ72"/>
+      <c r="AI72">
+        <v>142.5</v>
+      </c>
+      <c r="AJ72">
+        <f t="shared" si="113"/>
+        <v>22.299999999999997</v>
+      </c>
+      <c r="AK72">
+        <v>120.2</v>
+      </c>
+      <c r="AL72">
+        <v>695.87</v>
+      </c>
+      <c r="AM72">
+        <f t="shared" si="114"/>
+        <v>695.87</v>
+      </c>
+      <c r="AN72" s="50">
+        <f t="shared" si="115"/>
+        <v>1.3666628241827539</v>
+      </c>
+      <c r="AO72">
+        <v>1</v>
+      </c>
+      <c r="AP72">
+        <v>11</v>
+      </c>
+      <c r="AQ72" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR72">
+        <v>0</v>
+      </c>
+      <c r="AS72" t="s">
+        <v>180</v>
+      </c>
+      <c r="AT72">
+        <v>0</v>
+      </c>
+      <c r="AU72" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV72" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW72" t="s">
+        <v>33</v>
+      </c>
       <c r="AY72">
         <v>2</v>
+      </c>
+      <c r="AZ72" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:52" x14ac:dyDescent="0.3">
@@ -16635,7 +16829,7 @@
         <v>0</v>
       </c>
       <c r="AQ107" t="s">
-        <v>109</v>
+        <v>192</v>
       </c>
       <c r="AR107">
         <v>2.74</v>

</xml_diff>

<commit_message>
added new snakes from 2024, and updated some scripts
</commit_message>
<xml_diff>
--- a/Snake_captures.xlsx
+++ b/Snake_captures.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc9\Desktop\Marc\CREAF\Snake tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033E38D0-3FBB-4F79-A583-363FA0D86DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A6D092-466B-41A0-B765-6D092D25CDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{01147B77-2702-4854-93BF-07D9F62605BE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01147B77-2702-4854-93BF-07D9F62605BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Snakes" sheetId="1" r:id="rId1"/>
     <sheet name="Read_me" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Snakes!$A$1:$AX$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Snakes!$A$1:$AX$163</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1999" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2407" uniqueCount="207">
   <si>
     <t>Snake_ID</t>
   </si>
@@ -630,6 +630,39 @@
   <si>
     <t xml:space="preserve"> the tag is separated, and as the sanke didn't get out of the refuge, we can't determine its visual phenotype in the video. I think this snake is SN_1, as it is the only snake without tag in the behaviour bag, but I cannot confirm.</t>
   </si>
+  <si>
+    <t>Atzaró</t>
+  </si>
+  <si>
+    <t>Macias</t>
+  </si>
+  <si>
+    <t>Santa Eularia</t>
+  </si>
+  <si>
+    <t>Vives</t>
+  </si>
+  <si>
+    <t>Sunny (25%)</t>
+  </si>
+  <si>
+    <t>Sunny, Windy (5%)</t>
+  </si>
+  <si>
+    <t>N (rep)</t>
+  </si>
+  <si>
+    <t>Very windy day. Not tracked for the moment, as it is only used for head-out/body-out</t>
+  </si>
+  <si>
+    <t>Not tracked for the moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> as it is only used for head-out/body-out</t>
+  </si>
+  <si>
+    <t>Kids playing around making noise. Disturbing? Not tracked for the moment, as it is only used for head-out/body-out</t>
+  </si>
 </sst>
 </file>
 
@@ -723,10 +756,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -735,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -788,6 +830,12 @@
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1108,13 +1156,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E02FB2-7411-4C81-A76E-E8A0CC2B910F}">
-  <dimension ref="A1:AZ131"/>
+  <dimension ref="A1:BA163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO5" sqref="AO5"/>
+      <selection pane="bottomRight" activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1122,15 +1170,18 @@
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" customWidth="1"/>
     <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.5546875" style="20"/>
     <col min="22" max="22" width="11.5546875" style="26"/>
     <col min="23" max="23" width="11.5546875" style="20"/>
     <col min="24" max="24" width="11.5546875" style="26" customWidth="1"/>
     <col min="25" max="25" width="11.5546875" style="20"/>
-    <col min="26" max="27" width="11.5546875" style="26"/>
+    <col min="26" max="26" width="11.5546875" style="26"/>
     <col min="28" max="29" width="11.5546875" style="20"/>
-    <col min="30" max="36" width="11.5546875" style="26"/>
+    <col min="30" max="30" width="11.5546875" style="26"/>
+    <col min="32" max="36" width="11.5546875" style="26"/>
     <col min="41" max="42" width="11.5546875" style="26"/>
     <col min="43" max="43" width="15.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="11.5546875" customWidth="1"/>
@@ -1215,7 +1266,7 @@
       <c r="Z1" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="AA1" s="23" t="s">
+      <c r="AA1" s="5" t="s">
         <v>166</v>
       </c>
       <c r="AB1" s="17" t="s">
@@ -1227,7 +1278,7 @@
       <c r="AD1" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="AE1" s="23" t="s">
+      <c r="AE1" s="5" t="s">
         <v>167</v>
       </c>
       <c r="AF1" s="23" t="s">
@@ -17525,7 +17576,7 @@
         <v>45092</v>
       </c>
       <c r="K112">
-        <f t="shared" ref="K112:K131" si="162">J112-I112</f>
+        <f t="shared" ref="K112:K148" si="162">J112-I112</f>
         <v>3</v>
       </c>
       <c r="L112" s="7">
@@ -20091,7 +20142,9 @@
       <c r="F128" s="8">
         <v>4322215</v>
       </c>
-      <c r="G128" s="8"/>
+      <c r="G128" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="H128" s="8" t="s">
         <v>12</v>
       </c>
@@ -20236,7 +20289,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>12071</v>
       </c>
@@ -20398,7 +20451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:52" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:53" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="45">
         <v>12072</v>
       </c>
@@ -20560,7 +20613,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="131" spans="1:52" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="8">
         <v>202308</v>
       </c>
@@ -20575,6 +20628,9 @@
       </c>
       <c r="F131" s="8">
         <v>4309046</v>
+      </c>
+      <c r="G131" s="8" t="s">
+        <v>149</v>
       </c>
       <c r="H131" s="8" t="s">
         <v>96</v>
@@ -20719,8 +20775,3810 @@
         <v>126</v>
       </c>
     </row>
+    <row r="132" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>14237</v>
+      </c>
+      <c r="B132">
+        <v>1268</v>
+      </c>
+      <c r="C132" t="s">
+        <v>34</v>
+      </c>
+      <c r="D132" t="s">
+        <v>40</v>
+      </c>
+      <c r="E132" s="51">
+        <v>364908</v>
+      </c>
+      <c r="F132" s="52">
+        <v>4314575</v>
+      </c>
+      <c r="G132" t="s">
+        <v>148</v>
+      </c>
+      <c r="H132" t="s">
+        <v>199</v>
+      </c>
+      <c r="I132" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J132" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K132">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L132" s="7">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="M132" s="7">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="N132" s="7">
+        <v>0.45347222222222222</v>
+      </c>
+      <c r="O132">
+        <v>26.9</v>
+      </c>
+      <c r="P132">
+        <v>50.2</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>201</v>
+      </c>
+      <c r="R132" t="s">
+        <v>39</v>
+      </c>
+      <c r="S132" t="s">
+        <v>33</v>
+      </c>
+      <c r="T132" t="s">
+        <v>32</v>
+      </c>
+      <c r="U132" s="20">
+        <v>7.1759259259259259E-4</v>
+      </c>
+      <c r="V132" s="26">
+        <f t="shared" ref="V132:V163" si="190">U132</f>
+        <v>7.1759259259259259E-4</v>
+      </c>
+      <c r="W132" s="20">
+        <v>6.4583333333333333E-3</v>
+      </c>
+      <c r="X132" s="26">
+        <f>W132</f>
+        <v>6.4583333333333333E-3</v>
+      </c>
+      <c r="Y132" s="20">
+        <f>W132-U132</f>
+        <v>5.7407407407407407E-3</v>
+      </c>
+      <c r="Z132" s="26">
+        <f>Y132</f>
+        <v>5.7407407407407407E-3</v>
+      </c>
+      <c r="AA132">
+        <v>496</v>
+      </c>
+      <c r="AB132" s="20">
+        <v>9.3287037037037036E-3</v>
+      </c>
+      <c r="AC132" s="20">
+        <f>AB132-U132</f>
+        <v>8.611111111111111E-3</v>
+      </c>
+      <c r="AD132" s="26">
+        <f>AC132</f>
+        <v>8.611111111111111E-3</v>
+      </c>
+      <c r="AE132">
+        <v>744</v>
+      </c>
+      <c r="AF132" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG132">
+        <v>2019.3466800000001</v>
+      </c>
+      <c r="AH132">
+        <v>5881.8775387412497</v>
+      </c>
+      <c r="AI132"/>
+      <c r="AJ132"/>
+      <c r="AO132"/>
+      <c r="AP132"/>
+      <c r="AQ132"/>
+      <c r="AY132">
+        <v>2</v>
+      </c>
+      <c r="AZ132" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="133" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>12488</v>
+      </c>
+      <c r="B133">
+        <v>2184</v>
+      </c>
+      <c r="C133" t="s">
+        <v>34</v>
+      </c>
+      <c r="D133" t="s">
+        <v>198</v>
+      </c>
+      <c r="E133" s="51">
+        <v>372437</v>
+      </c>
+      <c r="F133" s="52">
+        <v>4315885</v>
+      </c>
+      <c r="G133" t="s">
+        <v>148</v>
+      </c>
+      <c r="H133" t="s">
+        <v>197</v>
+      </c>
+      <c r="I133" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J133" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K133">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="L133" s="7">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="M133" s="7">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="N133" s="7">
+        <v>0.45347222222222222</v>
+      </c>
+      <c r="O133">
+        <v>26.9</v>
+      </c>
+      <c r="P133">
+        <v>50.2</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>201</v>
+      </c>
+      <c r="R133" t="s">
+        <v>43</v>
+      </c>
+      <c r="S133" t="s">
+        <v>33</v>
+      </c>
+      <c r="T133" t="s">
+        <v>32</v>
+      </c>
+      <c r="U133" s="20">
+        <v>6.134259259259259E-4</v>
+      </c>
+      <c r="V133" s="26">
+        <f t="shared" si="190"/>
+        <v>6.134259259259259E-4</v>
+      </c>
+      <c r="W133" s="20">
+        <v>7.905092592592592E-3</v>
+      </c>
+      <c r="X133" s="26">
+        <f>W133</f>
+        <v>7.905092592592592E-3</v>
+      </c>
+      <c r="Y133" s="20">
+        <f>W133-U133</f>
+        <v>7.2916666666666659E-3</v>
+      </c>
+      <c r="Z133" s="26">
+        <f>Y133</f>
+        <v>7.2916666666666659E-3</v>
+      </c>
+      <c r="AA133">
+        <v>630</v>
+      </c>
+      <c r="AB133" s="20">
+        <v>1.6620370370370369E-2</v>
+      </c>
+      <c r="AC133" s="20">
+        <f>AB133-U133</f>
+        <v>1.6006944444444442E-2</v>
+      </c>
+      <c r="AD133" s="26">
+        <f>AC133</f>
+        <v>1.6006944444444442E-2</v>
+      </c>
+      <c r="AE133">
+        <v>1383</v>
+      </c>
+      <c r="AF133" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG133">
+        <v>2013.03809</v>
+      </c>
+      <c r="AH133">
+        <v>4354.2529517041203</v>
+      </c>
+      <c r="AI133"/>
+      <c r="AJ133"/>
+      <c r="AO133"/>
+      <c r="AP133"/>
+      <c r="AQ133"/>
+      <c r="AY133">
+        <v>2</v>
+      </c>
+      <c r="AZ133" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="134" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>12504</v>
+      </c>
+      <c r="B134">
+        <v>2224</v>
+      </c>
+      <c r="C134" t="s">
+        <v>34</v>
+      </c>
+      <c r="D134" t="s">
+        <v>198</v>
+      </c>
+      <c r="E134" s="51">
+        <v>369196</v>
+      </c>
+      <c r="F134" s="52">
+        <v>4325662</v>
+      </c>
+      <c r="G134" t="s">
+        <v>148</v>
+      </c>
+      <c r="H134" t="s">
+        <v>197</v>
+      </c>
+      <c r="I134" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J134" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K134">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="L134" s="7">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="M134" s="7">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="N134" s="7">
+        <v>0.45347222222222222</v>
+      </c>
+      <c r="O134">
+        <v>26.9</v>
+      </c>
+      <c r="P134">
+        <v>50.2</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>201</v>
+      </c>
+      <c r="R134" t="s">
+        <v>69</v>
+      </c>
+      <c r="S134" t="s">
+        <v>33</v>
+      </c>
+      <c r="T134" t="s">
+        <v>32</v>
+      </c>
+      <c r="U134" s="20">
+        <v>4.9768518518518521E-4</v>
+      </c>
+      <c r="V134" s="26">
+        <f t="shared" si="190"/>
+        <v>4.9768518518518521E-4</v>
+      </c>
+      <c r="W134" s="20">
+        <v>1.7048611111111112E-2</v>
+      </c>
+      <c r="X134" s="26">
+        <f>W134</f>
+        <v>1.7048611111111112E-2</v>
+      </c>
+      <c r="Y134" s="20">
+        <f>W134-U134</f>
+        <v>1.6550925925925927E-2</v>
+      </c>
+      <c r="Z134" s="26">
+        <f>Y134</f>
+        <v>1.6550925925925927E-2</v>
+      </c>
+      <c r="AA134">
+        <v>1430</v>
+      </c>
+      <c r="AB134" s="20">
+        <v>3.425925925925926E-2</v>
+      </c>
+      <c r="AC134" s="20">
+        <f>AB134-U134</f>
+        <v>3.3761574074074076E-2</v>
+      </c>
+      <c r="AD134" s="26">
+        <f>AC134</f>
+        <v>3.3761574074074076E-2</v>
+      </c>
+      <c r="AE134">
+        <v>2917</v>
+      </c>
+      <c r="AF134" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG134">
+        <v>2020.99243</v>
+      </c>
+      <c r="AH134">
+        <v>7035.7609244589103</v>
+      </c>
+      <c r="AI134"/>
+      <c r="AJ134"/>
+      <c r="AO134"/>
+      <c r="AP134"/>
+      <c r="AQ134"/>
+      <c r="AY134">
+        <v>2</v>
+      </c>
+      <c r="AZ134" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="135" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>12485</v>
+      </c>
+      <c r="B135">
+        <v>2038</v>
+      </c>
+      <c r="C135" t="s">
+        <v>34</v>
+      </c>
+      <c r="D135" t="s">
+        <v>196</v>
+      </c>
+      <c r="E135" s="51">
+        <v>371221</v>
+      </c>
+      <c r="F135" s="52">
+        <v>4319293</v>
+      </c>
+      <c r="G135" t="s">
+        <v>148</v>
+      </c>
+      <c r="H135" t="s">
+        <v>197</v>
+      </c>
+      <c r="I135" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J135" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L135" s="7">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="M135" s="7">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="N135" s="7">
+        <v>0.45347222222222222</v>
+      </c>
+      <c r="O135">
+        <v>26.9</v>
+      </c>
+      <c r="P135">
+        <v>50.2</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>201</v>
+      </c>
+      <c r="R135" t="s">
+        <v>44</v>
+      </c>
+      <c r="S135" t="s">
+        <v>33</v>
+      </c>
+      <c r="T135" t="s">
+        <v>32</v>
+      </c>
+      <c r="U135" s="20">
+        <v>5.4398148148148144E-4</v>
+      </c>
+      <c r="V135" s="26">
+        <f t="shared" si="190"/>
+        <v>5.4398148148148144E-4</v>
+      </c>
+      <c r="W135" t="s">
+        <v>109</v>
+      </c>
+      <c r="X135" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y135" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z135" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA135" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB135" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC135" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD135" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE135" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF135" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG135">
+        <v>2015.4209000000001</v>
+      </c>
+      <c r="AH135">
+        <v>2216.74578694108</v>
+      </c>
+      <c r="AI135"/>
+      <c r="AJ135"/>
+      <c r="AO135"/>
+      <c r="AP135"/>
+      <c r="AQ135"/>
+      <c r="AY135">
+        <v>2</v>
+      </c>
+      <c r="AZ135" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="136" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>14236</v>
+      </c>
+      <c r="B136">
+        <v>1271</v>
+      </c>
+      <c r="C136" t="s">
+        <v>34</v>
+      </c>
+      <c r="D136" t="s">
+        <v>40</v>
+      </c>
+      <c r="E136" s="51">
+        <v>365321</v>
+      </c>
+      <c r="F136" s="52">
+        <v>4313910</v>
+      </c>
+      <c r="G136" t="s">
+        <v>148</v>
+      </c>
+      <c r="H136" t="s">
+        <v>199</v>
+      </c>
+      <c r="I136" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J136" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K136">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L136" s="7">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="M136" s="7">
+        <v>0.53125</v>
+      </c>
+      <c r="N136" s="7">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="O136">
+        <v>31.3</v>
+      </c>
+      <c r="P136">
+        <v>42.2</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>123</v>
+      </c>
+      <c r="R136" t="s">
+        <v>39</v>
+      </c>
+      <c r="S136" t="s">
+        <v>33</v>
+      </c>
+      <c r="T136" t="s">
+        <v>32</v>
+      </c>
+      <c r="U136" s="20">
+        <v>3.7384259259259259E-3</v>
+      </c>
+      <c r="V136" s="26">
+        <f t="shared" si="190"/>
+        <v>3.7384259259259259E-3</v>
+      </c>
+      <c r="W136" s="20">
+        <v>8.2754629629629636E-3</v>
+      </c>
+      <c r="X136" s="26">
+        <f>W136</f>
+        <v>8.2754629629629636E-3</v>
+      </c>
+      <c r="Y136" s="20">
+        <f>W136-U136</f>
+        <v>4.5370370370370373E-3</v>
+      </c>
+      <c r="Z136" s="26">
+        <f>Y136</f>
+        <v>4.5370370370370373E-3</v>
+      </c>
+      <c r="AA136">
+        <v>392</v>
+      </c>
+      <c r="AB136" s="20">
+        <v>1.0636574074074074E-2</v>
+      </c>
+      <c r="AC136" s="20">
+        <f>AB136-U136</f>
+        <v>6.898148148148148E-3</v>
+      </c>
+      <c r="AD136" s="26">
+        <f>AC136</f>
+        <v>6.898148148148148E-3</v>
+      </c>
+      <c r="AE136">
+        <v>596</v>
+      </c>
+      <c r="AF136" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG136">
+        <v>2018.5125700000001</v>
+      </c>
+      <c r="AH136">
+        <v>5934.2469148699902</v>
+      </c>
+      <c r="AY136">
+        <v>2</v>
+      </c>
+      <c r="AZ136" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA136" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="137" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>12487</v>
+      </c>
+      <c r="B137">
+        <v>2183</v>
+      </c>
+      <c r="C137" t="s">
+        <v>34</v>
+      </c>
+      <c r="D137" t="s">
+        <v>198</v>
+      </c>
+      <c r="E137" s="51">
+        <v>372360</v>
+      </c>
+      <c r="F137" s="52">
+        <v>4315792</v>
+      </c>
+      <c r="G137" t="s">
+        <v>148</v>
+      </c>
+      <c r="H137" t="s">
+        <v>197</v>
+      </c>
+      <c r="I137" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J137" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K137">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="L137" s="7">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="M137" s="7">
+        <v>0.53125</v>
+      </c>
+      <c r="N137" s="7">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="O137">
+        <v>31.3</v>
+      </c>
+      <c r="P137">
+        <v>42.2</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>123</v>
+      </c>
+      <c r="R137" t="s">
+        <v>43</v>
+      </c>
+      <c r="S137" t="s">
+        <v>33</v>
+      </c>
+      <c r="T137" t="s">
+        <v>32</v>
+      </c>
+      <c r="U137" s="20">
+        <v>3.7037037037037038E-3</v>
+      </c>
+      <c r="V137" s="26">
+        <f t="shared" si="190"/>
+        <v>3.7037037037037038E-3</v>
+      </c>
+      <c r="W137" s="20">
+        <v>9.1550925925925931E-3</v>
+      </c>
+      <c r="X137" s="26">
+        <f>W137</f>
+        <v>9.1550925925925931E-3</v>
+      </c>
+      <c r="Y137" s="20">
+        <f>W137-U137</f>
+        <v>5.4513888888888893E-3</v>
+      </c>
+      <c r="Z137" s="26">
+        <f>Y137</f>
+        <v>5.4513888888888893E-3</v>
+      </c>
+      <c r="AA137">
+        <v>471</v>
+      </c>
+      <c r="AB137" s="20">
+        <v>1.2858796296296297E-2</v>
+      </c>
+      <c r="AC137" s="20">
+        <f>AB137-U137</f>
+        <v>9.1550925925925931E-3</v>
+      </c>
+      <c r="AD137" s="26">
+        <f>AC137</f>
+        <v>9.1550925925925931E-3</v>
+      </c>
+      <c r="AE137">
+        <v>791</v>
+      </c>
+      <c r="AF137" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG137">
+        <v>2013.5502899999899</v>
+      </c>
+      <c r="AH137">
+        <v>4514.5507831750501</v>
+      </c>
+      <c r="AY137">
+        <v>2</v>
+      </c>
+      <c r="AZ137" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA137" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="138" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>12480</v>
+      </c>
+      <c r="B138">
+        <v>2004</v>
+      </c>
+      <c r="C138" t="s">
+        <v>34</v>
+      </c>
+      <c r="D138" t="s">
+        <v>196</v>
+      </c>
+      <c r="E138" s="51">
+        <v>375064</v>
+      </c>
+      <c r="F138" s="52">
+        <v>4322654</v>
+      </c>
+      <c r="G138" t="s">
+        <v>148</v>
+      </c>
+      <c r="H138" t="s">
+        <v>197</v>
+      </c>
+      <c r="I138" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J138" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K138">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L138" s="7">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="M138" s="7">
+        <v>0.53125</v>
+      </c>
+      <c r="N138" s="7">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="O138">
+        <v>31.3</v>
+      </c>
+      <c r="P138">
+        <v>42.2</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>123</v>
+      </c>
+      <c r="R138" t="s">
+        <v>69</v>
+      </c>
+      <c r="S138" t="s">
+        <v>33</v>
+      </c>
+      <c r="T138" t="s">
+        <v>32</v>
+      </c>
+      <c r="U138" s="20">
+        <v>3.7962962962962963E-3</v>
+      </c>
+      <c r="V138" s="26">
+        <f t="shared" si="190"/>
+        <v>3.7962962962962963E-3</v>
+      </c>
+      <c r="W138" t="s">
+        <v>109</v>
+      </c>
+      <c r="X138" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y138" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z138" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA138" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB138" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC138" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD138" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE138" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF138" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG138">
+        <v>2017.97693</v>
+      </c>
+      <c r="AH138">
+        <v>7356.8859383323897</v>
+      </c>
+      <c r="AY138">
+        <v>2</v>
+      </c>
+      <c r="AZ138" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA138" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="139" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>14238</v>
+      </c>
+      <c r="B139">
+        <v>1277</v>
+      </c>
+      <c r="C139" t="s">
+        <v>34</v>
+      </c>
+      <c r="D139" t="s">
+        <v>40</v>
+      </c>
+      <c r="E139" s="51">
+        <v>365084</v>
+      </c>
+      <c r="F139" s="52">
+        <v>4315012</v>
+      </c>
+      <c r="G139" t="s">
+        <v>148</v>
+      </c>
+      <c r="H139" t="s">
+        <v>199</v>
+      </c>
+      <c r="I139" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J139" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K139">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L139" s="7">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="M139" s="7">
+        <v>0.53125</v>
+      </c>
+      <c r="N139" s="7">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="O139">
+        <v>31.3</v>
+      </c>
+      <c r="P139">
+        <v>42.2</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>123</v>
+      </c>
+      <c r="R139" t="s">
+        <v>44</v>
+      </c>
+      <c r="S139" t="s">
+        <v>33</v>
+      </c>
+      <c r="T139" t="s">
+        <v>32</v>
+      </c>
+      <c r="U139" s="20">
+        <v>3.8425925925925928E-3</v>
+      </c>
+      <c r="V139" s="26">
+        <f t="shared" si="190"/>
+        <v>3.8425925925925928E-3</v>
+      </c>
+      <c r="W139" s="20">
+        <v>1.8622685185185187E-2</v>
+      </c>
+      <c r="X139" s="26">
+        <f t="shared" ref="X139:X148" si="191">W139</f>
+        <v>1.8622685185185187E-2</v>
+      </c>
+      <c r="Y139" s="20">
+        <f t="shared" ref="Y139:Y148" si="192">W139-U139</f>
+        <v>1.4780092592592595E-2</v>
+      </c>
+      <c r="Z139" s="26">
+        <f t="shared" ref="Z139:Z148" si="193">Y139</f>
+        <v>1.4780092592592595E-2</v>
+      </c>
+      <c r="AA139">
+        <v>1277</v>
+      </c>
+      <c r="AB139" s="20">
+        <v>2.6458333333333334E-2</v>
+      </c>
+      <c r="AC139" s="20">
+        <f>AB139-U139</f>
+        <v>2.2615740740740742E-2</v>
+      </c>
+      <c r="AD139" s="26">
+        <f>AC139</f>
+        <v>2.2615740740740742E-2</v>
+      </c>
+      <c r="AE139">
+        <v>1954</v>
+      </c>
+      <c r="AF139" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG139">
+        <v>2016.3063999999899</v>
+      </c>
+      <c r="AH139">
+        <v>5351.6637298022997</v>
+      </c>
+      <c r="AY139">
+        <v>2</v>
+      </c>
+      <c r="AZ139" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA139" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="140" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>12479</v>
+      </c>
+      <c r="B140">
+        <v>2003</v>
+      </c>
+      <c r="C140" t="s">
+        <v>34</v>
+      </c>
+      <c r="D140" t="s">
+        <v>196</v>
+      </c>
+      <c r="E140" s="51">
+        <v>375237</v>
+      </c>
+      <c r="F140" s="52">
+        <v>4322339</v>
+      </c>
+      <c r="G140" t="s">
+        <v>148</v>
+      </c>
+      <c r="H140" t="s">
+        <v>197</v>
+      </c>
+      <c r="I140" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J140" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K140">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L140" s="7">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="M140" s="7">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="N140" s="7">
+        <v>0.64027777777777772</v>
+      </c>
+      <c r="O140">
+        <v>32.9</v>
+      </c>
+      <c r="P140">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>105</v>
+      </c>
+      <c r="R140" t="s">
+        <v>39</v>
+      </c>
+      <c r="S140" t="s">
+        <v>33</v>
+      </c>
+      <c r="T140" t="s">
+        <v>32</v>
+      </c>
+      <c r="U140" s="20">
+        <v>3.5879629629629629E-4</v>
+      </c>
+      <c r="V140" s="26">
+        <f t="shared" si="190"/>
+        <v>3.5879629629629629E-4</v>
+      </c>
+      <c r="W140" s="20">
+        <v>7.905092592592592E-3</v>
+      </c>
+      <c r="X140" s="26">
+        <f t="shared" si="191"/>
+        <v>7.905092592592592E-3</v>
+      </c>
+      <c r="Y140" s="20">
+        <f t="shared" si="192"/>
+        <v>7.5462962962962957E-3</v>
+      </c>
+      <c r="Z140" s="26">
+        <f t="shared" si="193"/>
+        <v>7.5462962962962957E-3</v>
+      </c>
+      <c r="AA140">
+        <v>652</v>
+      </c>
+      <c r="AB140" s="20">
+        <v>1.2164351851851852E-2</v>
+      </c>
+      <c r="AC140" s="20">
+        <f>AB140-U140</f>
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="AD140" s="26">
+        <f>AC140</f>
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="AE140">
+        <v>1020</v>
+      </c>
+      <c r="AF140" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG140">
+        <v>2016.9019800000001</v>
+      </c>
+      <c r="AH140">
+        <v>7095.0310070925698</v>
+      </c>
+      <c r="AY140">
+        <v>2</v>
+      </c>
+      <c r="AZ140" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA140" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="141" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>12503</v>
+      </c>
+      <c r="B141">
+        <v>2211</v>
+      </c>
+      <c r="C141" t="s">
+        <v>34</v>
+      </c>
+      <c r="D141" t="s">
+        <v>198</v>
+      </c>
+      <c r="E141" s="51">
+        <v>367419</v>
+      </c>
+      <c r="F141" s="52">
+        <v>4325171</v>
+      </c>
+      <c r="G141" t="s">
+        <v>148</v>
+      </c>
+      <c r="H141" t="s">
+        <v>197</v>
+      </c>
+      <c r="I141" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J141" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K141">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="L141" s="7">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="M141" s="7">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="N141" s="7">
+        <v>0.64027777777777772</v>
+      </c>
+      <c r="O141">
+        <v>32.9</v>
+      </c>
+      <c r="P141">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>105</v>
+      </c>
+      <c r="R141" t="s">
+        <v>43</v>
+      </c>
+      <c r="S141" t="s">
+        <v>33</v>
+      </c>
+      <c r="T141" t="s">
+        <v>32</v>
+      </c>
+      <c r="U141" s="20">
+        <v>3.0092592592592595E-4</v>
+      </c>
+      <c r="V141" s="26">
+        <f t="shared" si="190"/>
+        <v>3.0092592592592595E-4</v>
+      </c>
+      <c r="W141" s="20">
+        <v>1.0590277777777778E-2</v>
+      </c>
+      <c r="X141" s="26">
+        <f t="shared" si="191"/>
+        <v>1.0590277777777778E-2</v>
+      </c>
+      <c r="Y141" s="20">
+        <f t="shared" si="192"/>
+        <v>1.0289351851851852E-2</v>
+      </c>
+      <c r="Z141" s="26">
+        <f t="shared" si="193"/>
+        <v>1.0289351851851852E-2</v>
+      </c>
+      <c r="AA141">
+        <v>889</v>
+      </c>
+      <c r="AB141" s="20">
+        <v>1.292824074074074E-2</v>
+      </c>
+      <c r="AC141" s="20">
+        <f>AB141-U141</f>
+        <v>1.2627314814814813E-2</v>
+      </c>
+      <c r="AD141" s="26">
+        <f>AC141</f>
+        <v>1.2627314814814813E-2</v>
+      </c>
+      <c r="AE141">
+        <v>1091</v>
+      </c>
+      <c r="AF141" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG141">
+        <v>2021.3741500000001</v>
+      </c>
+      <c r="AH141">
+        <v>6726.8218383447302</v>
+      </c>
+      <c r="AY141">
+        <v>2</v>
+      </c>
+      <c r="AZ141" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA141" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="142" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>12482</v>
+      </c>
+      <c r="B142">
+        <v>2022</v>
+      </c>
+      <c r="C142" t="s">
+        <v>34</v>
+      </c>
+      <c r="D142" t="s">
+        <v>196</v>
+      </c>
+      <c r="E142" s="51">
+        <v>372034</v>
+      </c>
+      <c r="F142" s="52">
+        <v>4320680</v>
+      </c>
+      <c r="G142" t="s">
+        <v>148</v>
+      </c>
+      <c r="H142" t="s">
+        <v>197</v>
+      </c>
+      <c r="I142" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J142" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K142">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L142" s="7">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="M142" s="7">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="N142" s="7">
+        <v>0.64027777777777772</v>
+      </c>
+      <c r="O142">
+        <v>32.9</v>
+      </c>
+      <c r="P142">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>105</v>
+      </c>
+      <c r="R142" t="s">
+        <v>69</v>
+      </c>
+      <c r="S142" t="s">
+        <v>33</v>
+      </c>
+      <c r="T142" t="s">
+        <v>32</v>
+      </c>
+      <c r="U142" s="20">
+        <v>4.1666666666666669E-4</v>
+      </c>
+      <c r="V142" s="26">
+        <f t="shared" si="190"/>
+        <v>4.1666666666666669E-4</v>
+      </c>
+      <c r="W142" s="20">
+        <v>3.8657407407407408E-3</v>
+      </c>
+      <c r="X142" s="26">
+        <f t="shared" si="191"/>
+        <v>3.8657407407407408E-3</v>
+      </c>
+      <c r="Y142" s="20">
+        <f t="shared" si="192"/>
+        <v>3.449074074074074E-3</v>
+      </c>
+      <c r="Z142" s="26">
+        <f t="shared" si="193"/>
+        <v>3.449074074074074E-3</v>
+      </c>
+      <c r="AA142">
+        <v>289</v>
+      </c>
+      <c r="AB142" s="20">
+        <v>5.162037037037037E-3</v>
+      </c>
+      <c r="AC142" s="20">
+        <f>AB142-U142</f>
+        <v>4.7453703703703703E-3</v>
+      </c>
+      <c r="AD142" s="26">
+        <f>AC142</f>
+        <v>4.7453703703703703E-3</v>
+      </c>
+      <c r="AE142">
+        <v>410</v>
+      </c>
+      <c r="AF142" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG142">
+        <v>2016.7569599999899</v>
+      </c>
+      <c r="AH142">
+        <v>3750.8110018563102</v>
+      </c>
+      <c r="AY142">
+        <v>2</v>
+      </c>
+      <c r="AZ142" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA142" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="143" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>12484</v>
+      </c>
+      <c r="B143">
+        <v>2031</v>
+      </c>
+      <c r="C143" t="s">
+        <v>34</v>
+      </c>
+      <c r="D143" t="s">
+        <v>196</v>
+      </c>
+      <c r="E143" s="51">
+        <v>374176</v>
+      </c>
+      <c r="F143" s="52">
+        <v>4316922</v>
+      </c>
+      <c r="G143" t="s">
+        <v>148</v>
+      </c>
+      <c r="H143" t="s">
+        <v>197</v>
+      </c>
+      <c r="I143" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J143" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K143">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L143" s="7">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="M143" s="7">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="N143" s="7">
+        <v>0.64027777777777772</v>
+      </c>
+      <c r="O143">
+        <v>32.9</v>
+      </c>
+      <c r="P143">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>105</v>
+      </c>
+      <c r="R143" t="s">
+        <v>44</v>
+      </c>
+      <c r="S143" t="s">
+        <v>33</v>
+      </c>
+      <c r="T143" t="s">
+        <v>32</v>
+      </c>
+      <c r="U143" s="20">
+        <v>4.6296296296296298E-4</v>
+      </c>
+      <c r="V143" s="26">
+        <f t="shared" si="190"/>
+        <v>4.6296296296296298E-4</v>
+      </c>
+      <c r="W143" s="20">
+        <v>9.3055555555555548E-3</v>
+      </c>
+      <c r="X143" s="26">
+        <f t="shared" si="191"/>
+        <v>9.3055555555555548E-3</v>
+      </c>
+      <c r="Y143" s="20">
+        <f t="shared" si="192"/>
+        <v>8.8425925925925911E-3</v>
+      </c>
+      <c r="Z143" s="26">
+        <f t="shared" si="193"/>
+        <v>8.8425925925925911E-3</v>
+      </c>
+      <c r="AA143">
+        <v>764</v>
+      </c>
+      <c r="AB143" s="20">
+        <v>1.0439814814814815E-2</v>
+      </c>
+      <c r="AC143" s="20">
+        <f>AB143-U143</f>
+        <v>9.9768518518518513E-3</v>
+      </c>
+      <c r="AD143" s="26">
+        <f>AC143</f>
+        <v>9.9768518518518513E-3</v>
+      </c>
+      <c r="AE143">
+        <v>862</v>
+      </c>
+      <c r="AF143" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG143">
+        <v>2014.4504400000001</v>
+      </c>
+      <c r="AH143">
+        <v>5431.0692328075402</v>
+      </c>
+      <c r="AY143">
+        <v>2</v>
+      </c>
+      <c r="AZ143" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA143" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="144" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>12483</v>
+      </c>
+      <c r="B144">
+        <v>2023</v>
+      </c>
+      <c r="C144" t="s">
+        <v>34</v>
+      </c>
+      <c r="D144" t="s">
+        <v>196</v>
+      </c>
+      <c r="E144" s="51">
+        <v>372205</v>
+      </c>
+      <c r="F144" s="52">
+        <v>4320330</v>
+      </c>
+      <c r="G144" t="s">
+        <v>148</v>
+      </c>
+      <c r="H144" t="s">
+        <v>197</v>
+      </c>
+      <c r="I144" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J144" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K144">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L144" s="7">
+        <v>0.72291666666666665</v>
+      </c>
+      <c r="M144" s="7">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="N144" s="7">
+        <v>0.72777777777777775</v>
+      </c>
+      <c r="O144">
+        <v>30.1</v>
+      </c>
+      <c r="P144">
+        <v>41.7</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>85</v>
+      </c>
+      <c r="R144" t="s">
+        <v>39</v>
+      </c>
+      <c r="S144" t="s">
+        <v>33</v>
+      </c>
+      <c r="T144" t="s">
+        <v>32</v>
+      </c>
+      <c r="U144" s="20">
+        <v>2.6041666666666665E-3</v>
+      </c>
+      <c r="V144" s="26">
+        <f t="shared" si="190"/>
+        <v>2.6041666666666665E-3</v>
+      </c>
+      <c r="W144" s="20">
+        <v>2.2303240740740742E-2</v>
+      </c>
+      <c r="X144" s="26">
+        <f t="shared" si="191"/>
+        <v>2.2303240740740742E-2</v>
+      </c>
+      <c r="Y144" s="20">
+        <f t="shared" si="192"/>
+        <v>1.9699074074074074E-2</v>
+      </c>
+      <c r="Z144" s="26">
+        <f t="shared" si="193"/>
+        <v>1.9699074074074074E-2</v>
+      </c>
+      <c r="AA144">
+        <v>1702</v>
+      </c>
+      <c r="AB144" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC144" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD144" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE144" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF144" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG144">
+        <v>2015.6724899999899</v>
+      </c>
+      <c r="AH144">
+        <v>3505.0090424359701</v>
+      </c>
+      <c r="AY144">
+        <v>2</v>
+      </c>
+      <c r="AZ144" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA144" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="145" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>12481</v>
+      </c>
+      <c r="B145">
+        <v>2008</v>
+      </c>
+      <c r="C145" t="s">
+        <v>34</v>
+      </c>
+      <c r="D145" t="s">
+        <v>196</v>
+      </c>
+      <c r="E145" s="51">
+        <v>373917</v>
+      </c>
+      <c r="F145" s="52">
+        <v>4320504</v>
+      </c>
+      <c r="G145" t="s">
+        <v>148</v>
+      </c>
+      <c r="H145" t="s">
+        <v>197</v>
+      </c>
+      <c r="I145" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J145" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K145">
+        <f t="shared" si="162"/>
+        <v>3</v>
+      </c>
+      <c r="L145" s="7">
+        <v>0.72291666666666665</v>
+      </c>
+      <c r="M145" s="7">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="N145" s="7">
+        <v>0.72777777777777775</v>
+      </c>
+      <c r="O145">
+        <v>30.1</v>
+      </c>
+      <c r="P145">
+        <v>41.7</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>85</v>
+      </c>
+      <c r="R145" t="s">
+        <v>43</v>
+      </c>
+      <c r="S145" t="s">
+        <v>33</v>
+      </c>
+      <c r="T145" t="s">
+        <v>32</v>
+      </c>
+      <c r="U145" s="20">
+        <v>2.5462962962962965E-3</v>
+      </c>
+      <c r="V145" s="26">
+        <f t="shared" si="190"/>
+        <v>2.5462962962962965E-3</v>
+      </c>
+      <c r="W145" s="20">
+        <v>1.0497685185185185E-2</v>
+      </c>
+      <c r="X145" s="26">
+        <f t="shared" si="191"/>
+        <v>1.0497685185185185E-2</v>
+      </c>
+      <c r="Y145" s="20">
+        <f t="shared" si="192"/>
+        <v>7.951388888888888E-3</v>
+      </c>
+      <c r="Z145" s="26">
+        <f t="shared" si="193"/>
+        <v>7.951388888888888E-3</v>
+      </c>
+      <c r="AA145">
+        <v>687</v>
+      </c>
+      <c r="AB145" s="20">
+        <v>1.5520833333333333E-2</v>
+      </c>
+      <c r="AC145" s="20">
+        <f>AB145-U145</f>
+        <v>1.2974537037037036E-2</v>
+      </c>
+      <c r="AD145" s="26">
+        <f>AC145</f>
+        <v>1.2974537037037036E-2</v>
+      </c>
+      <c r="AE145">
+        <v>1121</v>
+      </c>
+      <c r="AF145" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG145">
+        <v>2018.6908000000001</v>
+      </c>
+      <c r="AH145">
+        <v>5216.5177038905204</v>
+      </c>
+      <c r="AY145">
+        <v>2</v>
+      </c>
+      <c r="AZ145" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA145" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="146" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>12486</v>
+      </c>
+      <c r="B146">
+        <v>2180</v>
+      </c>
+      <c r="C146" t="s">
+        <v>34</v>
+      </c>
+      <c r="D146" t="s">
+        <v>198</v>
+      </c>
+      <c r="E146" s="51">
+        <v>372723</v>
+      </c>
+      <c r="F146" s="52">
+        <v>4314766</v>
+      </c>
+      <c r="G146" t="s">
+        <v>148</v>
+      </c>
+      <c r="H146" t="s">
+        <v>197</v>
+      </c>
+      <c r="I146" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J146" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K146">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="L146" s="7">
+        <v>0.72291666666666665</v>
+      </c>
+      <c r="M146" s="7">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="N146" s="7">
+        <v>0.72777777777777775</v>
+      </c>
+      <c r="O146">
+        <v>30.1</v>
+      </c>
+      <c r="P146">
+        <v>41.7</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>85</v>
+      </c>
+      <c r="R146" t="s">
+        <v>69</v>
+      </c>
+      <c r="S146" t="s">
+        <v>33</v>
+      </c>
+      <c r="T146" t="s">
+        <v>32</v>
+      </c>
+      <c r="U146" s="20">
+        <v>2.673611111111111E-3</v>
+      </c>
+      <c r="V146" s="26">
+        <f t="shared" si="190"/>
+        <v>2.673611111111111E-3</v>
+      </c>
+      <c r="W146" s="20">
+        <v>3.7905092592592594E-2</v>
+      </c>
+      <c r="X146" s="26">
+        <f t="shared" si="191"/>
+        <v>3.7905092592592594E-2</v>
+      </c>
+      <c r="Y146" s="20">
+        <f t="shared" si="192"/>
+        <v>3.5231481481481482E-2</v>
+      </c>
+      <c r="Z146" s="26">
+        <f t="shared" si="193"/>
+        <v>3.5231481481481482E-2</v>
+      </c>
+      <c r="AA146">
+        <v>3044</v>
+      </c>
+      <c r="AB146" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC146" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD146" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE146" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF146" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG146">
+        <v>2016.5406499999899</v>
+      </c>
+      <c r="AH146">
+        <v>5392.7844314882204</v>
+      </c>
+      <c r="AY146">
+        <v>2</v>
+      </c>
+      <c r="AZ146" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA146" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="147" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>12489</v>
+      </c>
+      <c r="B147">
+        <v>2188</v>
+      </c>
+      <c r="C147" t="s">
+        <v>34</v>
+      </c>
+      <c r="D147" t="s">
+        <v>198</v>
+      </c>
+      <c r="E147" s="51">
+        <v>370295</v>
+      </c>
+      <c r="F147" s="52">
+        <v>4318018</v>
+      </c>
+      <c r="G147" t="s">
+        <v>148</v>
+      </c>
+      <c r="H147" t="s">
+        <v>197</v>
+      </c>
+      <c r="I147" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J147" s="4">
+        <v>45452</v>
+      </c>
+      <c r="K147">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="L147" s="7">
+        <v>0.72291666666666665</v>
+      </c>
+      <c r="M147" s="7">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="N147" s="7">
+        <v>0.72777777777777775</v>
+      </c>
+      <c r="O147">
+        <v>30.1</v>
+      </c>
+      <c r="P147">
+        <v>41.7</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>85</v>
+      </c>
+      <c r="R147" t="s">
+        <v>44</v>
+      </c>
+      <c r="S147" t="s">
+        <v>33</v>
+      </c>
+      <c r="T147" t="s">
+        <v>32</v>
+      </c>
+      <c r="U147" s="20">
+        <v>2.7662037037037039E-3</v>
+      </c>
+      <c r="V147" s="26">
+        <f t="shared" si="190"/>
+        <v>2.7662037037037039E-3</v>
+      </c>
+      <c r="W147" s="20">
+        <v>5.9375000000000001E-3</v>
+      </c>
+      <c r="X147" s="26">
+        <f t="shared" si="191"/>
+        <v>5.9375000000000001E-3</v>
+      </c>
+      <c r="Y147" s="20">
+        <f t="shared" si="192"/>
+        <v>3.1712962962962962E-3</v>
+      </c>
+      <c r="Z147" s="26">
+        <f t="shared" si="193"/>
+        <v>3.1712962962962962E-3</v>
+      </c>
+      <c r="AA147">
+        <v>274</v>
+      </c>
+      <c r="AB147" s="20">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AC147" s="20">
+        <f>AB147-U147</f>
+        <v>4.7337962962962958E-3</v>
+      </c>
+      <c r="AD147" s="26">
+        <f>AC147</f>
+        <v>4.7337962962962958E-3</v>
+      </c>
+      <c r="AE147">
+        <v>409</v>
+      </c>
+      <c r="AF147" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG147">
+        <v>2014.7381600000001</v>
+      </c>
+      <c r="AH147">
+        <v>1574.4920471851001</v>
+      </c>
+      <c r="AY147">
+        <v>2</v>
+      </c>
+      <c r="AZ147" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA147" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="148" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>12482</v>
+      </c>
+      <c r="B148">
+        <v>2022</v>
+      </c>
+      <c r="C148" t="s">
+        <v>34</v>
+      </c>
+      <c r="D148" t="s">
+        <v>196</v>
+      </c>
+      <c r="E148" s="51">
+        <v>372034</v>
+      </c>
+      <c r="F148" s="52">
+        <v>4320680</v>
+      </c>
+      <c r="G148" t="s">
+        <v>148</v>
+      </c>
+      <c r="H148" t="s">
+        <v>197</v>
+      </c>
+      <c r="I148" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J148" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K148">
+        <f t="shared" si="162"/>
+        <v>4</v>
+      </c>
+      <c r="L148" s="7">
+        <v>0.39791666666666664</v>
+      </c>
+      <c r="M148" s="7">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="N148" s="7">
+        <v>0.40625</v>
+      </c>
+      <c r="O148">
+        <v>26.2</v>
+      </c>
+      <c r="P148">
+        <v>58.7</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>80</v>
+      </c>
+      <c r="R148" t="s">
+        <v>39</v>
+      </c>
+      <c r="S148" t="s">
+        <v>33</v>
+      </c>
+      <c r="T148" t="s">
+        <v>33</v>
+      </c>
+      <c r="U148" s="20">
+        <v>3.1250000000000001E-4</v>
+      </c>
+      <c r="V148" s="26">
+        <f t="shared" si="190"/>
+        <v>3.1250000000000001E-4</v>
+      </c>
+      <c r="W148" s="20">
+        <v>1.0231481481481482E-2</v>
+      </c>
+      <c r="X148" s="26">
+        <f t="shared" si="191"/>
+        <v>1.0231481481481482E-2</v>
+      </c>
+      <c r="Y148" s="20">
+        <f t="shared" si="192"/>
+        <v>9.9189814814814817E-3</v>
+      </c>
+      <c r="Z148" s="26">
+        <f t="shared" si="193"/>
+        <v>9.9189814814814817E-3</v>
+      </c>
+      <c r="AA148">
+        <v>857</v>
+      </c>
+      <c r="AB148" s="20">
+        <v>1.2812499999999999E-2</v>
+      </c>
+      <c r="AC148" s="20">
+        <f>AB148-U148</f>
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="AD148" s="26">
+        <f>AC148</f>
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="AE148">
+        <v>1080</v>
+      </c>
+      <c r="AF148" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG148">
+        <v>2016.7569599999899</v>
+      </c>
+      <c r="AH148">
+        <v>3750.8110018563102</v>
+      </c>
+      <c r="AY148">
+        <v>2</v>
+      </c>
+      <c r="AZ148" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="149" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>12484</v>
+      </c>
+      <c r="B149">
+        <v>2031</v>
+      </c>
+      <c r="C149" t="s">
+        <v>34</v>
+      </c>
+      <c r="D149" t="s">
+        <v>196</v>
+      </c>
+      <c r="E149" s="51">
+        <v>374176</v>
+      </c>
+      <c r="F149" s="52">
+        <v>4316922</v>
+      </c>
+      <c r="G149" t="s">
+        <v>148</v>
+      </c>
+      <c r="H149" t="s">
+        <v>197</v>
+      </c>
+      <c r="I149" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J149" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K149">
+        <f t="shared" ref="K149:K163" si="194">J149-I149</f>
+        <v>4</v>
+      </c>
+      <c r="L149" s="7">
+        <v>0.39791666666666664</v>
+      </c>
+      <c r="M149" s="7">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="N149" s="7">
+        <v>0.40625</v>
+      </c>
+      <c r="O149">
+        <v>26.2</v>
+      </c>
+      <c r="P149">
+        <v>58.7</v>
+      </c>
+      <c r="Q149" t="s">
+        <v>80</v>
+      </c>
+      <c r="R149" t="s">
+        <v>43</v>
+      </c>
+      <c r="S149" t="s">
+        <v>33</v>
+      </c>
+      <c r="T149" t="s">
+        <v>33</v>
+      </c>
+      <c r="U149" s="20">
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="V149" s="26">
+        <f t="shared" si="190"/>
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="W149" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="X149" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y149" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z149" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA149" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB149" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC149" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD149" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE149" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF149" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG149">
+        <v>2014.4504400000001</v>
+      </c>
+      <c r="AH149">
+        <v>5431.0692328075402</v>
+      </c>
+      <c r="AY149">
+        <v>2</v>
+      </c>
+      <c r="AZ149" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="150" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>12485</v>
+      </c>
+      <c r="B150">
+        <v>2038</v>
+      </c>
+      <c r="C150" t="s">
+        <v>34</v>
+      </c>
+      <c r="D150" t="s">
+        <v>196</v>
+      </c>
+      <c r="E150" s="51">
+        <v>371221</v>
+      </c>
+      <c r="F150" s="52">
+        <v>4319293</v>
+      </c>
+      <c r="G150" t="s">
+        <v>148</v>
+      </c>
+      <c r="H150" t="s">
+        <v>197</v>
+      </c>
+      <c r="I150" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J150" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K150">
+        <f t="shared" si="194"/>
+        <v>4</v>
+      </c>
+      <c r="L150" s="7">
+        <v>0.39791666666666664</v>
+      </c>
+      <c r="M150" s="7">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="N150" s="7">
+        <v>0.40625</v>
+      </c>
+      <c r="O150">
+        <v>26.2</v>
+      </c>
+      <c r="P150">
+        <v>58.7</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>80</v>
+      </c>
+      <c r="R150" t="s">
+        <v>69</v>
+      </c>
+      <c r="S150" t="s">
+        <v>33</v>
+      </c>
+      <c r="T150" t="s">
+        <v>33</v>
+      </c>
+      <c r="U150" s="20">
+        <v>4.6296296296296298E-4</v>
+      </c>
+      <c r="V150" s="26">
+        <f t="shared" si="190"/>
+        <v>4.6296296296296298E-4</v>
+      </c>
+      <c r="W150" s="20">
+        <v>6.1689814814814819E-3</v>
+      </c>
+      <c r="X150" s="26">
+        <f>W150</f>
+        <v>6.1689814814814819E-3</v>
+      </c>
+      <c r="Y150" s="20">
+        <f>W150-U150</f>
+        <v>5.7060185185185191E-3</v>
+      </c>
+      <c r="Z150" s="26">
+        <f>Y150</f>
+        <v>5.7060185185185191E-3</v>
+      </c>
+      <c r="AA150">
+        <v>493</v>
+      </c>
+      <c r="AB150" s="20">
+        <v>1.0972222222222222E-2</v>
+      </c>
+      <c r="AC150" s="20">
+        <f>AB150-U150</f>
+        <v>1.0509259259259258E-2</v>
+      </c>
+      <c r="AD150" s="26">
+        <f>AC150</f>
+        <v>1.0509259259259258E-2</v>
+      </c>
+      <c r="AE150">
+        <v>908</v>
+      </c>
+      <c r="AF150" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG150">
+        <v>2015.4209000000001</v>
+      </c>
+      <c r="AH150">
+        <v>2216.74578694108</v>
+      </c>
+      <c r="AY150">
+        <v>2</v>
+      </c>
+      <c r="AZ150" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="151" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>12504</v>
+      </c>
+      <c r="B151">
+        <v>2224</v>
+      </c>
+      <c r="C151" t="s">
+        <v>34</v>
+      </c>
+      <c r="D151" t="s">
+        <v>198</v>
+      </c>
+      <c r="E151" s="51">
+        <v>369196</v>
+      </c>
+      <c r="F151" s="52">
+        <v>4325662</v>
+      </c>
+      <c r="G151" t="s">
+        <v>148</v>
+      </c>
+      <c r="H151" t="s">
+        <v>197</v>
+      </c>
+      <c r="I151" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J151" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K151">
+        <f t="shared" si="194"/>
+        <v>3</v>
+      </c>
+      <c r="L151" s="7">
+        <v>0.39791666666666664</v>
+      </c>
+      <c r="M151" s="7">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="N151" s="7">
+        <v>0.40625</v>
+      </c>
+      <c r="O151">
+        <v>26.2</v>
+      </c>
+      <c r="P151">
+        <v>58.7</v>
+      </c>
+      <c r="Q151" t="s">
+        <v>80</v>
+      </c>
+      <c r="R151" t="s">
+        <v>44</v>
+      </c>
+      <c r="S151" t="s">
+        <v>33</v>
+      </c>
+      <c r="T151" t="s">
+        <v>33</v>
+      </c>
+      <c r="U151" s="20">
+        <v>4.9768518518518521E-4</v>
+      </c>
+      <c r="V151" s="26">
+        <f t="shared" si="190"/>
+        <v>4.9768518518518521E-4</v>
+      </c>
+      <c r="W151" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="X151" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y151" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z151" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA151" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB151" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC151" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD151" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE151" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF151" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG151">
+        <v>2020.99243</v>
+      </c>
+      <c r="AH151">
+        <v>7035.7609244589103</v>
+      </c>
+      <c r="AY151">
+        <v>2</v>
+      </c>
+      <c r="AZ151" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="152" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>14236</v>
+      </c>
+      <c r="B152">
+        <v>1271</v>
+      </c>
+      <c r="C152" t="s">
+        <v>34</v>
+      </c>
+      <c r="D152" t="s">
+        <v>40</v>
+      </c>
+      <c r="E152" s="51">
+        <v>365321</v>
+      </c>
+      <c r="F152" s="52">
+        <v>4313910</v>
+      </c>
+      <c r="G152" t="s">
+        <v>148</v>
+      </c>
+      <c r="H152" t="s">
+        <v>199</v>
+      </c>
+      <c r="I152" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J152" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K152">
+        <f t="shared" si="194"/>
+        <v>4</v>
+      </c>
+      <c r="L152" s="7">
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="M152" s="7">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="N152" s="7">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="O152">
+        <v>27.8</v>
+      </c>
+      <c r="P152">
+        <v>58.5</v>
+      </c>
+      <c r="Q152" t="s">
+        <v>85</v>
+      </c>
+      <c r="R152" t="s">
+        <v>39</v>
+      </c>
+      <c r="S152" t="s">
+        <v>33</v>
+      </c>
+      <c r="T152" t="s">
+        <v>33</v>
+      </c>
+      <c r="U152" s="20">
+        <v>5.0925925925925921E-4</v>
+      </c>
+      <c r="V152" s="26">
+        <f t="shared" si="190"/>
+        <v>5.0925925925925921E-4</v>
+      </c>
+      <c r="W152" s="20">
+        <v>1.0891203703703703E-2</v>
+      </c>
+      <c r="X152" s="26">
+        <f>W152</f>
+        <v>1.0891203703703703E-2</v>
+      </c>
+      <c r="Y152" s="20">
+        <f>W152-U152</f>
+        <v>1.0381944444444444E-2</v>
+      </c>
+      <c r="Z152" s="26">
+        <f>Y152</f>
+        <v>1.0381944444444444E-2</v>
+      </c>
+      <c r="AA152">
+        <v>897</v>
+      </c>
+      <c r="AB152" s="20">
+        <v>1.7708333333333333E-2</v>
+      </c>
+      <c r="AC152" s="20">
+        <f>AB152-U152</f>
+        <v>1.7199074074074075E-2</v>
+      </c>
+      <c r="AD152" s="26">
+        <f>AC152</f>
+        <v>1.7199074074074075E-2</v>
+      </c>
+      <c r="AE152">
+        <v>1486</v>
+      </c>
+      <c r="AF152" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG152">
+        <v>2018.5125700000001</v>
+      </c>
+      <c r="AH152">
+        <v>5934.2469148699902</v>
+      </c>
+      <c r="AY152">
+        <v>2</v>
+      </c>
+      <c r="AZ152" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA152" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="153" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>12503</v>
+      </c>
+      <c r="B153">
+        <v>2211</v>
+      </c>
+      <c r="C153" t="s">
+        <v>34</v>
+      </c>
+      <c r="D153" t="s">
+        <v>198</v>
+      </c>
+      <c r="E153" s="51">
+        <v>367419</v>
+      </c>
+      <c r="F153" s="52">
+        <v>4325171</v>
+      </c>
+      <c r="G153" t="s">
+        <v>148</v>
+      </c>
+      <c r="H153" t="s">
+        <v>197</v>
+      </c>
+      <c r="I153" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J153" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K153">
+        <f t="shared" si="194"/>
+        <v>3</v>
+      </c>
+      <c r="L153" s="7">
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="M153" s="7">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="N153" s="7">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="O153">
+        <v>27.8</v>
+      </c>
+      <c r="P153">
+        <v>58.5</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>85</v>
+      </c>
+      <c r="R153" t="s">
+        <v>43</v>
+      </c>
+      <c r="S153" t="s">
+        <v>33</v>
+      </c>
+      <c r="T153" t="s">
+        <v>33</v>
+      </c>
+      <c r="U153" s="20">
+        <v>4.6296296296296298E-4</v>
+      </c>
+      <c r="V153" s="26">
+        <f t="shared" si="190"/>
+        <v>4.6296296296296298E-4</v>
+      </c>
+      <c r="W153" s="20">
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="X153" s="26">
+        <f>W153</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="Y153" s="20">
+        <f>W153-U153</f>
+        <v>1.2870370370370371E-2</v>
+      </c>
+      <c r="Z153" s="26">
+        <f>Y153</f>
+        <v>1.2870370370370371E-2</v>
+      </c>
+      <c r="AA153">
+        <v>1112</v>
+      </c>
+      <c r="AB153" s="20">
+        <v>1.8067129629629631E-2</v>
+      </c>
+      <c r="AC153" s="20">
+        <f>AB153-U153</f>
+        <v>1.7604166666666667E-2</v>
+      </c>
+      <c r="AD153" s="26">
+        <f>AC153</f>
+        <v>1.7604166666666667E-2</v>
+      </c>
+      <c r="AE153">
+        <v>1521</v>
+      </c>
+      <c r="AF153" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG153">
+        <v>2021.3741500000001</v>
+      </c>
+      <c r="AH153">
+        <v>6726.8218383447302</v>
+      </c>
+      <c r="AY153">
+        <v>2</v>
+      </c>
+      <c r="AZ153" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA153" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="154" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>12488</v>
+      </c>
+      <c r="B154">
+        <v>2184</v>
+      </c>
+      <c r="C154" t="s">
+        <v>34</v>
+      </c>
+      <c r="D154" t="s">
+        <v>198</v>
+      </c>
+      <c r="E154" s="51">
+        <v>372437</v>
+      </c>
+      <c r="F154" s="52">
+        <v>4315885</v>
+      </c>
+      <c r="G154" t="s">
+        <v>148</v>
+      </c>
+      <c r="H154" t="s">
+        <v>197</v>
+      </c>
+      <c r="I154" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J154" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K154">
+        <f t="shared" si="194"/>
+        <v>3</v>
+      </c>
+      <c r="L154" s="7">
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="M154" s="7">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="N154" s="7">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="O154">
+        <v>27.8</v>
+      </c>
+      <c r="P154">
+        <v>58.5</v>
+      </c>
+      <c r="Q154" t="s">
+        <v>85</v>
+      </c>
+      <c r="R154" t="s">
+        <v>69</v>
+      </c>
+      <c r="S154" t="s">
+        <v>33</v>
+      </c>
+      <c r="T154" t="s">
+        <v>33</v>
+      </c>
+      <c r="U154" s="20">
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="V154" s="26">
+        <f t="shared" si="190"/>
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="W154" s="20">
+        <v>1.7372685185185185E-2</v>
+      </c>
+      <c r="X154" s="26">
+        <f>W154</f>
+        <v>1.7372685185185185E-2</v>
+      </c>
+      <c r="Y154" s="20">
+        <f>W154-U154</f>
+        <v>1.7002314814814814E-2</v>
+      </c>
+      <c r="Z154" s="26">
+        <f>Y154</f>
+        <v>1.7002314814814814E-2</v>
+      </c>
+      <c r="AA154">
+        <v>1469</v>
+      </c>
+      <c r="AB154" s="20">
+        <v>2.4062500000000001E-2</v>
+      </c>
+      <c r="AC154" s="20">
+        <f>AB154-U154</f>
+        <v>2.3692129629629629E-2</v>
+      </c>
+      <c r="AD154" s="26">
+        <f>AC154</f>
+        <v>2.3692129629629629E-2</v>
+      </c>
+      <c r="AE154">
+        <v>2047</v>
+      </c>
+      <c r="AF154" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG154">
+        <v>2013.03809</v>
+      </c>
+      <c r="AH154">
+        <v>4354.2529517041203</v>
+      </c>
+      <c r="AY154">
+        <v>2</v>
+      </c>
+      <c r="AZ154" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA154" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="155" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>12489</v>
+      </c>
+      <c r="B155">
+        <v>2188</v>
+      </c>
+      <c r="C155" t="s">
+        <v>34</v>
+      </c>
+      <c r="D155" t="s">
+        <v>198</v>
+      </c>
+      <c r="E155" s="51">
+        <v>370295</v>
+      </c>
+      <c r="F155" s="52">
+        <v>4318018</v>
+      </c>
+      <c r="G155" t="s">
+        <v>148</v>
+      </c>
+      <c r="H155" t="s">
+        <v>197</v>
+      </c>
+      <c r="I155" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J155" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K155">
+        <f t="shared" si="194"/>
+        <v>3</v>
+      </c>
+      <c r="L155" s="7">
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="M155" s="7">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="N155" s="7">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="O155">
+        <v>27.8</v>
+      </c>
+      <c r="P155">
+        <v>58.5</v>
+      </c>
+      <c r="Q155" t="s">
+        <v>85</v>
+      </c>
+      <c r="R155" t="s">
+        <v>44</v>
+      </c>
+      <c r="S155" t="s">
+        <v>33</v>
+      </c>
+      <c r="T155" t="s">
+        <v>33</v>
+      </c>
+      <c r="U155" s="20">
+        <v>4.0509259259259258E-4</v>
+      </c>
+      <c r="V155" s="26">
+        <f t="shared" si="190"/>
+        <v>4.0509259259259258E-4</v>
+      </c>
+      <c r="W155" s="20">
+        <v>5.6597222222222222E-3</v>
+      </c>
+      <c r="X155" s="26">
+        <f>W155</f>
+        <v>5.6597222222222222E-3</v>
+      </c>
+      <c r="Y155" s="20">
+        <f>W155-U155</f>
+        <v>5.2546296296296299E-3</v>
+      </c>
+      <c r="Z155" s="26">
+        <f>Y155</f>
+        <v>5.2546296296296299E-3</v>
+      </c>
+      <c r="AA155">
+        <v>454</v>
+      </c>
+      <c r="AB155" s="20">
+        <v>8.7152777777777784E-3</v>
+      </c>
+      <c r="AC155" s="20">
+        <f>AB155-U155</f>
+        <v>8.3101851851851861E-3</v>
+      </c>
+      <c r="AD155" s="26">
+        <f>AC155</f>
+        <v>8.3101851851851861E-3</v>
+      </c>
+      <c r="AE155">
+        <v>718</v>
+      </c>
+      <c r="AF155" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG155">
+        <v>2014.7381600000001</v>
+      </c>
+      <c r="AH155">
+        <v>1574.4920471851001</v>
+      </c>
+      <c r="AY155">
+        <v>2</v>
+      </c>
+      <c r="AZ155" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA155" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="156" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>12481</v>
+      </c>
+      <c r="B156">
+        <v>2008</v>
+      </c>
+      <c r="C156" t="s">
+        <v>34</v>
+      </c>
+      <c r="D156" t="s">
+        <v>196</v>
+      </c>
+      <c r="E156" s="51">
+        <v>373917</v>
+      </c>
+      <c r="F156" s="52">
+        <v>4320504</v>
+      </c>
+      <c r="G156" t="s">
+        <v>148</v>
+      </c>
+      <c r="H156" t="s">
+        <v>197</v>
+      </c>
+      <c r="I156" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J156" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K156">
+        <f t="shared" si="194"/>
+        <v>4</v>
+      </c>
+      <c r="L156" s="7">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="M156" s="7">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="N156" s="7">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="O156">
+        <v>31.2</v>
+      </c>
+      <c r="P156">
+        <v>49.3</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>200</v>
+      </c>
+      <c r="R156" t="s">
+        <v>39</v>
+      </c>
+      <c r="S156" t="s">
+        <v>33</v>
+      </c>
+      <c r="T156" t="s">
+        <v>33</v>
+      </c>
+      <c r="U156" s="20">
+        <v>2.6620370370370372E-4</v>
+      </c>
+      <c r="V156" s="26">
+        <f t="shared" si="190"/>
+        <v>2.6620370370370372E-4</v>
+      </c>
+      <c r="W156" s="20">
+        <v>4.2476851851851851E-3</v>
+      </c>
+      <c r="X156" s="26">
+        <f>W156</f>
+        <v>4.2476851851851851E-3</v>
+      </c>
+      <c r="Y156" s="20">
+        <f>W156-U156</f>
+        <v>3.9814814814814817E-3</v>
+      </c>
+      <c r="Z156" s="26">
+        <f>Y156</f>
+        <v>3.9814814814814817E-3</v>
+      </c>
+      <c r="AA156">
+        <v>344</v>
+      </c>
+      <c r="AB156" s="20">
+        <v>1.8553240740740742E-2</v>
+      </c>
+      <c r="AC156" s="20">
+        <f>AB156-U156</f>
+        <v>1.8287037037037039E-2</v>
+      </c>
+      <c r="AD156" s="26">
+        <f>AC156</f>
+        <v>1.8287037037037039E-2</v>
+      </c>
+      <c r="AE156">
+        <v>1580</v>
+      </c>
+      <c r="AF156" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG156">
+        <v>2018.6908000000001</v>
+      </c>
+      <c r="AH156">
+        <v>5216.5177038905204</v>
+      </c>
+      <c r="AY156">
+        <v>2</v>
+      </c>
+      <c r="AZ156" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA156" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="157" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>12480</v>
+      </c>
+      <c r="B157">
+        <v>2004</v>
+      </c>
+      <c r="C157" t="s">
+        <v>34</v>
+      </c>
+      <c r="D157" t="s">
+        <v>196</v>
+      </c>
+      <c r="E157" s="51">
+        <v>375064</v>
+      </c>
+      <c r="F157" s="52">
+        <v>4322654</v>
+      </c>
+      <c r="G157" t="s">
+        <v>148</v>
+      </c>
+      <c r="H157" t="s">
+        <v>197</v>
+      </c>
+      <c r="I157" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J157" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K157">
+        <f t="shared" si="194"/>
+        <v>4</v>
+      </c>
+      <c r="L157" s="7">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="M157" s="7">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="N157" s="7">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="O157">
+        <v>31.2</v>
+      </c>
+      <c r="P157">
+        <v>49.3</v>
+      </c>
+      <c r="Q157" t="s">
+        <v>200</v>
+      </c>
+      <c r="R157" t="s">
+        <v>43</v>
+      </c>
+      <c r="S157" t="s">
+        <v>33</v>
+      </c>
+      <c r="T157" t="s">
+        <v>33</v>
+      </c>
+      <c r="U157" s="20">
+        <v>3.1250000000000001E-4</v>
+      </c>
+      <c r="V157" s="26">
+        <f t="shared" si="190"/>
+        <v>3.1250000000000001E-4</v>
+      </c>
+      <c r="W157" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="X157" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y157" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z157" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA157" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB157" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC157" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD157" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE157" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF157" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG157">
+        <v>2017.97693</v>
+      </c>
+      <c r="AH157">
+        <v>7356.8859383323897</v>
+      </c>
+      <c r="AY157">
+        <v>2</v>
+      </c>
+      <c r="AZ157" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA157" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="158" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>12486</v>
+      </c>
+      <c r="B158">
+        <v>2180</v>
+      </c>
+      <c r="C158" t="s">
+        <v>34</v>
+      </c>
+      <c r="D158" t="s">
+        <v>198</v>
+      </c>
+      <c r="E158" s="51">
+        <v>372723</v>
+      </c>
+      <c r="F158" s="52">
+        <v>4314766</v>
+      </c>
+      <c r="G158" t="s">
+        <v>148</v>
+      </c>
+      <c r="H158" t="s">
+        <v>197</v>
+      </c>
+      <c r="I158" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J158" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K158">
+        <f t="shared" si="194"/>
+        <v>3</v>
+      </c>
+      <c r="L158" s="7">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="M158" s="7">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="N158" s="7">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="O158">
+        <v>31.2</v>
+      </c>
+      <c r="P158">
+        <v>49.3</v>
+      </c>
+      <c r="Q158" t="s">
+        <v>200</v>
+      </c>
+      <c r="R158" t="s">
+        <v>69</v>
+      </c>
+      <c r="S158" t="s">
+        <v>33</v>
+      </c>
+      <c r="T158" t="s">
+        <v>33</v>
+      </c>
+      <c r="U158" s="20">
+        <v>3.5879629629629629E-4</v>
+      </c>
+      <c r="V158" s="26">
+        <f t="shared" si="190"/>
+        <v>3.5879629629629629E-4</v>
+      </c>
+      <c r="W158" s="20">
+        <v>1.3344907407407408E-2</v>
+      </c>
+      <c r="X158" s="26">
+        <f>W158</f>
+        <v>1.3344907407407408E-2</v>
+      </c>
+      <c r="Y158" s="20">
+        <f>W158-U158</f>
+        <v>1.2986111111111111E-2</v>
+      </c>
+      <c r="Z158" s="26">
+        <f>Y158</f>
+        <v>1.2986111111111111E-2</v>
+      </c>
+      <c r="AA158">
+        <v>1122</v>
+      </c>
+      <c r="AB158" s="20">
+        <v>1.3958333333333333E-2</v>
+      </c>
+      <c r="AC158" s="20">
+        <f>AB158-U158</f>
+        <v>1.3599537037037037E-2</v>
+      </c>
+      <c r="AD158" s="26">
+        <f>AC158</f>
+        <v>1.3599537037037037E-2</v>
+      </c>
+      <c r="AE158">
+        <v>1175</v>
+      </c>
+      <c r="AF158" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG158">
+        <v>2016.5406499999899</v>
+      </c>
+      <c r="AH158">
+        <v>5392.7844314882204</v>
+      </c>
+      <c r="AY158">
+        <v>2</v>
+      </c>
+      <c r="AZ158" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA158" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="159" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>12483</v>
+      </c>
+      <c r="B159">
+        <v>2023</v>
+      </c>
+      <c r="C159" t="s">
+        <v>34</v>
+      </c>
+      <c r="D159" t="s">
+        <v>196</v>
+      </c>
+      <c r="E159" s="51">
+        <v>372205</v>
+      </c>
+      <c r="F159" s="52">
+        <v>4320330</v>
+      </c>
+      <c r="G159" t="s">
+        <v>148</v>
+      </c>
+      <c r="H159" t="s">
+        <v>197</v>
+      </c>
+      <c r="I159" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J159" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K159">
+        <f t="shared" si="194"/>
+        <v>4</v>
+      </c>
+      <c r="L159" s="7">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="M159" s="7">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="N159" s="7">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="O159">
+        <v>31.2</v>
+      </c>
+      <c r="P159">
+        <v>49.3</v>
+      </c>
+      <c r="Q159" t="s">
+        <v>200</v>
+      </c>
+      <c r="R159" t="s">
+        <v>44</v>
+      </c>
+      <c r="S159" t="s">
+        <v>33</v>
+      </c>
+      <c r="T159" t="s">
+        <v>33</v>
+      </c>
+      <c r="U159" s="20">
+        <v>3.9351851851851852E-4</v>
+      </c>
+      <c r="V159" s="26">
+        <f t="shared" si="190"/>
+        <v>3.9351851851851852E-4</v>
+      </c>
+      <c r="W159" s="20">
+        <v>2.3020833333333334E-2</v>
+      </c>
+      <c r="X159" s="26">
+        <f>W159</f>
+        <v>2.3020833333333334E-2</v>
+      </c>
+      <c r="Y159" s="20">
+        <f>W159-U159</f>
+        <v>2.2627314814814815E-2</v>
+      </c>
+      <c r="Z159" s="26">
+        <f>Y159</f>
+        <v>2.2627314814814815E-2</v>
+      </c>
+      <c r="AA159">
+        <v>1955</v>
+      </c>
+      <c r="AB159" s="20">
+        <v>2.4606481481481483E-2</v>
+      </c>
+      <c r="AC159" s="20">
+        <f>AB159-U159</f>
+        <v>2.4212962962962964E-2</v>
+      </c>
+      <c r="AD159" s="26">
+        <f>AC159</f>
+        <v>2.4212962962962964E-2</v>
+      </c>
+      <c r="AE159">
+        <v>2092</v>
+      </c>
+      <c r="AF159" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG159">
+        <v>2015.6724899999899</v>
+      </c>
+      <c r="AH159">
+        <v>3505.0090424359701</v>
+      </c>
+      <c r="AY159">
+        <v>2</v>
+      </c>
+      <c r="AZ159" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA159" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="160" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>12479</v>
+      </c>
+      <c r="B160">
+        <v>2003</v>
+      </c>
+      <c r="C160" t="s">
+        <v>34</v>
+      </c>
+      <c r="D160" t="s">
+        <v>196</v>
+      </c>
+      <c r="E160" s="51">
+        <v>375237</v>
+      </c>
+      <c r="F160" s="52">
+        <v>4322339</v>
+      </c>
+      <c r="G160" t="s">
+        <v>148</v>
+      </c>
+      <c r="H160" t="s">
+        <v>197</v>
+      </c>
+      <c r="I160" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J160" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K160">
+        <f t="shared" si="194"/>
+        <v>4</v>
+      </c>
+      <c r="L160" s="7">
+        <v>0.69166666666666665</v>
+      </c>
+      <c r="M160" s="7">
+        <v>0.69861111111111107</v>
+      </c>
+      <c r="N160" s="7">
+        <v>0.70208333333333328</v>
+      </c>
+      <c r="O160">
+        <v>27.1</v>
+      </c>
+      <c r="P160">
+        <v>58.7</v>
+      </c>
+      <c r="Q160" t="s">
+        <v>53</v>
+      </c>
+      <c r="R160" t="s">
+        <v>39</v>
+      </c>
+      <c r="S160" t="s">
+        <v>33</v>
+      </c>
+      <c r="T160" t="s">
+        <v>33</v>
+      </c>
+      <c r="U160" s="20">
+        <v>6.5972222222222224E-4</v>
+      </c>
+      <c r="V160" s="26">
+        <f t="shared" si="190"/>
+        <v>6.5972222222222224E-4</v>
+      </c>
+      <c r="W160" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="X160" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y160" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z160" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA160" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB160" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC160" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD160" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE160" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF160" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG160">
+        <v>2016.9019800000001</v>
+      </c>
+      <c r="AH160">
+        <v>7095.0310070925698</v>
+      </c>
+      <c r="AY160">
+        <v>2</v>
+      </c>
+      <c r="AZ160" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA160" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="161" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>14237</v>
+      </c>
+      <c r="B161">
+        <v>1268</v>
+      </c>
+      <c r="C161" t="s">
+        <v>34</v>
+      </c>
+      <c r="D161" t="s">
+        <v>40</v>
+      </c>
+      <c r="E161" s="51">
+        <v>364908</v>
+      </c>
+      <c r="F161" s="52">
+        <v>4314575</v>
+      </c>
+      <c r="G161" t="s">
+        <v>148</v>
+      </c>
+      <c r="H161" t="s">
+        <v>199</v>
+      </c>
+      <c r="I161" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J161" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K161">
+        <f t="shared" si="194"/>
+        <v>4</v>
+      </c>
+      <c r="L161" s="7">
+        <v>0.69166666666666665</v>
+      </c>
+      <c r="M161" s="7">
+        <v>0.69861111111111107</v>
+      </c>
+      <c r="N161" s="7">
+        <v>0.70208333333333328</v>
+      </c>
+      <c r="O161">
+        <v>27.1</v>
+      </c>
+      <c r="P161">
+        <v>58.7</v>
+      </c>
+      <c r="Q161" t="s">
+        <v>53</v>
+      </c>
+      <c r="R161" t="s">
+        <v>43</v>
+      </c>
+      <c r="S161" t="s">
+        <v>33</v>
+      </c>
+      <c r="T161" t="s">
+        <v>33</v>
+      </c>
+      <c r="U161" s="20">
+        <v>6.134259259259259E-4</v>
+      </c>
+      <c r="V161" s="26">
+        <f t="shared" si="190"/>
+        <v>6.134259259259259E-4</v>
+      </c>
+      <c r="W161" s="20">
+        <v>5.1273148148148146E-3</v>
+      </c>
+      <c r="X161" s="26">
+        <f>W161</f>
+        <v>5.1273148148148146E-3</v>
+      </c>
+      <c r="Y161" s="20">
+        <f>W161-U161</f>
+        <v>4.5138888888888885E-3</v>
+      </c>
+      <c r="Z161" s="26">
+        <f>Y161</f>
+        <v>4.5138888888888885E-3</v>
+      </c>
+      <c r="AA161">
+        <v>390</v>
+      </c>
+      <c r="AB161" s="20">
+        <v>1.2581018518518519E-2</v>
+      </c>
+      <c r="AC161" s="20">
+        <f>AB161-U161</f>
+        <v>1.1967592592592594E-2</v>
+      </c>
+      <c r="AD161" s="26">
+        <f>AC161</f>
+        <v>1.1967592592592594E-2</v>
+      </c>
+      <c r="AE161">
+        <v>1034</v>
+      </c>
+      <c r="AF161" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG161">
+        <v>2019.3466800000001</v>
+      </c>
+      <c r="AH161">
+        <v>5881.8775387412497</v>
+      </c>
+      <c r="AY161">
+        <v>2</v>
+      </c>
+      <c r="AZ161" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA161" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="162" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>14238</v>
+      </c>
+      <c r="B162">
+        <v>1277</v>
+      </c>
+      <c r="C162" t="s">
+        <v>34</v>
+      </c>
+      <c r="D162" t="s">
+        <v>40</v>
+      </c>
+      <c r="E162" s="51">
+        <v>365084</v>
+      </c>
+      <c r="F162" s="52">
+        <v>4315012</v>
+      </c>
+      <c r="G162" t="s">
+        <v>148</v>
+      </c>
+      <c r="H162" t="s">
+        <v>199</v>
+      </c>
+      <c r="I162" s="4">
+        <v>45449</v>
+      </c>
+      <c r="J162" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K162">
+        <f t="shared" si="194"/>
+        <v>4</v>
+      </c>
+      <c r="L162" s="7">
+        <v>0.69166666666666665</v>
+      </c>
+      <c r="M162" s="7">
+        <v>0.69861111111111107</v>
+      </c>
+      <c r="N162" s="7">
+        <v>0.70208333333333328</v>
+      </c>
+      <c r="O162">
+        <v>27.1</v>
+      </c>
+      <c r="P162">
+        <v>58.7</v>
+      </c>
+      <c r="Q162" t="s">
+        <v>53</v>
+      </c>
+      <c r="R162" t="s">
+        <v>69</v>
+      </c>
+      <c r="S162" t="s">
+        <v>33</v>
+      </c>
+      <c r="T162" t="s">
+        <v>33</v>
+      </c>
+      <c r="U162" s="20">
+        <v>7.6388888888888893E-4</v>
+      </c>
+      <c r="V162" s="26">
+        <f t="shared" si="190"/>
+        <v>7.6388888888888893E-4</v>
+      </c>
+      <c r="W162" s="20">
+        <v>1.7175925925925924E-2</v>
+      </c>
+      <c r="X162" s="26">
+        <f>W162</f>
+        <v>1.7175925925925924E-2</v>
+      </c>
+      <c r="Y162" s="20">
+        <f>W162-U162</f>
+        <v>1.6412037037037034E-2</v>
+      </c>
+      <c r="Z162" s="26">
+        <f>Y162</f>
+        <v>1.6412037037037034E-2</v>
+      </c>
+      <c r="AA162">
+        <v>1418</v>
+      </c>
+      <c r="AB162" s="20">
+        <v>2.4930555555555556E-2</v>
+      </c>
+      <c r="AC162" s="20">
+        <f>AB162-U162</f>
+        <v>2.4166666666666666E-2</v>
+      </c>
+      <c r="AD162" s="26">
+        <f>AC162</f>
+        <v>2.4166666666666666E-2</v>
+      </c>
+      <c r="AE162">
+        <v>2088</v>
+      </c>
+      <c r="AF162" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG162">
+        <v>2016.3063999999899</v>
+      </c>
+      <c r="AH162">
+        <v>5351.6637298022997</v>
+      </c>
+      <c r="AY162">
+        <v>2</v>
+      </c>
+      <c r="AZ162" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA162" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="163" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>12487</v>
+      </c>
+      <c r="B163">
+        <v>2183</v>
+      </c>
+      <c r="C163" t="s">
+        <v>34</v>
+      </c>
+      <c r="D163" t="s">
+        <v>198</v>
+      </c>
+      <c r="E163" s="51">
+        <v>372360</v>
+      </c>
+      <c r="F163" s="52">
+        <v>4315792</v>
+      </c>
+      <c r="G163" t="s">
+        <v>148</v>
+      </c>
+      <c r="H163" t="s">
+        <v>197</v>
+      </c>
+      <c r="I163" s="4">
+        <v>45450</v>
+      </c>
+      <c r="J163" s="4">
+        <v>45453</v>
+      </c>
+      <c r="K163">
+        <f t="shared" si="194"/>
+        <v>3</v>
+      </c>
+      <c r="L163" s="7">
+        <v>0.69166666666666665</v>
+      </c>
+      <c r="M163" s="7">
+        <v>0.69861111111111107</v>
+      </c>
+      <c r="N163" s="7">
+        <v>0.70208333333333328</v>
+      </c>
+      <c r="O163">
+        <v>27.1</v>
+      </c>
+      <c r="P163">
+        <v>58.7</v>
+      </c>
+      <c r="Q163" t="s">
+        <v>53</v>
+      </c>
+      <c r="R163" t="s">
+        <v>44</v>
+      </c>
+      <c r="S163" t="s">
+        <v>33</v>
+      </c>
+      <c r="T163" t="s">
+        <v>33</v>
+      </c>
+      <c r="U163" s="20">
+        <v>7.1759259259259259E-4</v>
+      </c>
+      <c r="V163" s="26">
+        <f t="shared" si="190"/>
+        <v>7.1759259259259259E-4</v>
+      </c>
+      <c r="W163" s="20">
+        <v>1.1666666666666667E-2</v>
+      </c>
+      <c r="X163" s="26">
+        <f>W163</f>
+        <v>1.1666666666666667E-2</v>
+      </c>
+      <c r="Y163" s="20">
+        <f>W163-U163</f>
+        <v>1.0949074074074075E-2</v>
+      </c>
+      <c r="Z163" s="26">
+        <f>Y163</f>
+        <v>1.0949074074074075E-2</v>
+      </c>
+      <c r="AA163">
+        <v>946</v>
+      </c>
+      <c r="AB163" s="20">
+        <v>1.8171296296296297E-2</v>
+      </c>
+      <c r="AC163" s="20">
+        <f>AB163-U163</f>
+        <v>1.7453703703703704E-2</v>
+      </c>
+      <c r="AD163" s="26">
+        <f>AC163</f>
+        <v>1.7453703703703704E-2</v>
+      </c>
+      <c r="AE163">
+        <v>1508</v>
+      </c>
+      <c r="AF163" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG163">
+        <v>2013.5502899999899</v>
+      </c>
+      <c r="AH163">
+        <v>4514.5507831750501</v>
+      </c>
+      <c r="AY163">
+        <v>2</v>
+      </c>
+      <c r="AZ163" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA163" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AX131" xr:uid="{63E02FB2-7411-4C81-A76E-E8A0CC2B910F}"/>
+  <autoFilter ref="A1:AX163" xr:uid="{63E02FB2-7411-4C81-A76E-E8A0CC2B910F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CJ64">
     <sortCondition ref="J2:J64"/>
     <sortCondition ref="L2:L64"/>

</xml_diff>